<commit_message>
added Product Register module
</commit_message>
<xml_diff>
--- a/tests/artifact/data/Mobile-ProductRegister.data.xlsx
+++ b/tests/artifact/data/Mobile-ProductRegister.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="231">
   <si>
     <t>login.screen</t>
   </si>
@@ -184,7 +184,7 @@
     <t>org.open</t>
   </si>
   <si>
-    <t>(//button[text()=' Open '])[104]</t>
+    <t>(//button[text()=' Open '])[99]</t>
   </si>
   <si>
     <t>org.hamburger</t>
@@ -622,7 +622,7 @@
     <t>pr.Invoice.hyperlink</t>
   </si>
   <si>
-    <t>//div[@class='mt-2']/div/table/tbody/tr[1]/td[2]/div/a/div</t>
+    <t>//div[@class='mt-2']/div/table/tbody/tr[2]/td[2]/div/a/div</t>
   </si>
   <si>
     <t>Invoice.name.heading</t>
@@ -704,6 +704,30 @@
   </si>
   <si>
     <t>//*[text()=' Credit Note']</t>
+  </si>
+  <si>
+    <t>Filter.nonselect.result</t>
+  </si>
+  <si>
+    <t>//div[@class='table-border-dark table-responsive-sm']/table/tbody/tr/td/div/h4</t>
+  </si>
+  <si>
+    <t>Product.values</t>
+  </si>
+  <si>
+    <t>Study Notes</t>
+  </si>
+  <si>
+    <t>search.field.value</t>
+  </si>
+  <si>
+    <t>3/SL-24</t>
+  </si>
+  <si>
+    <t>filter.button</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/section/div[3]/div/button</t>
   </si>
 </sst>
 </file>
@@ -1818,10 +1842,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C116"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2760,6 +2784,38 @@
         <v>222</v>
       </c>
     </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">

</xml_diff>